<commit_message>
Auto-committed on 2023/06/02 週五 11:31:19.42
</commit_message>
<xml_diff>
--- a/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
+++ b/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A9F5AF-C722-48F8-9FB4-CDDE73CAF3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="暫收款日餘額前後差異比較表" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,29 +375,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/11 週二 18:04:03.46
</commit_message>
<xml_diff>
--- a/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
+++ b/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A9F5AF-C722-48F8-9FB4-CDDE73CAF3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97014376-B5DC-491B-9C1F-E2BF3F0ABE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="暫收款日餘額前後差異比較表" sheetId="1" r:id="rId1"/>
@@ -20,37 +20,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>會計備份日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戶名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今日暫收款支票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今日暫收款非支票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>昨日暫收款支票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>昨日暫收款非支票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>會計日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>會計備份日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今日暫收款支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今日暫收款非支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>昨日暫收款支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>昨日暫收款非支票</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -94,8 +98,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -379,45 +389,50 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9" style="2"/>
+    <col min="4" max="4" width="17.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/17 週一 17:08:39.22
</commit_message>
<xml_diff>
--- a/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
+++ b/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97014376-B5DC-491B-9C1F-E2BF3F0ABE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF00551-22F8-4DEC-9C5A-C9C87DF0D597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,9 +388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Auto-committed on 2023/07/25 週二 11:42:26.11
</commit_message>
<xml_diff>
--- a/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
+++ b/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF00551-22F8-4DEC-9C5A-C9C87DF0D597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D929D60F-D887-406F-9D06-FE40960F4C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>會計備份日</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,10 +47,6 @@
   </si>
   <si>
     <t>昨日暫收款非支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>~</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -388,7 +384,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
@@ -404,11 +402,9 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Auto-committed on 2023/08/01 週二 11:43:26.84
</commit_message>
<xml_diff>
--- a/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
+++ b/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D929D60F-D887-406F-9D06-FE40960F4C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249D6589-2E73-4714-AEF7-A4B6A64C24AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="暫收款日餘額前後差異比較表" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>會計備份日</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,24 +34,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>今日暫收款支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今日暫收款非支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>昨日暫收款支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>昨日暫收款非支票</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>會計日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>額度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暫收款非支票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暫收款支票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今日</t>
+  </si>
+  <si>
+    <t>昨日</t>
   </si>
 </sst>
 </file>
@@ -382,51 +384,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9" style="2"/>
-    <col min="4" max="4" width="17.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="2"/>
+    <col min="3" max="4" width="9" style="2"/>
+    <col min="5" max="5" width="17.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/08/02 週三 16:52:43.81
</commit_message>
<xml_diff>
--- a/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
+++ b/Program/Other/L9139_底稿_暫收款日餘額前後差異比較表.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249D6589-2E73-4714-AEF7-A4B6A64C24AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECFF2CA-CD8E-4E09-AC53-091627A4243A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,8 @@
     <t>今日</t>
   </si>
   <si>
-    <t>昨日</t>
+    <t>前日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -387,7 +388,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>